<commit_message>
[Checkpoint] Clinic constraints & new form w/ working algorithm.
</commit_message>
<xml_diff>
--- a/Clinic Sign-Up Prototype_2.xlsx
+++ b/Clinic Sign-Up Prototype_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\Desktop\Clinics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9293A77D-C146-4E9D-98C4-8C4D9D61C7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBBF7CC-E1AA-4118-B090-7DB3E15E70A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="-120" windowWidth="27945" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="-120" windowWidth="27945" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="626">
   <si>
     <t>ID</t>
   </si>
@@ -1929,52 +1929,55 @@
     <t>4/25 from 6-7:30 (CoH);No Dates Available / Not Interested;4/19 from 5-6:30 (Calvert);4/26 from 5-6:30 (Calvert);4/5 from 5:00-6:30 pm (Calvert)</t>
   </si>
   <si>
-    <t>Stephanie Sorenson,Phyllis Davis</t>
-  </si>
-  <si>
-    <t>John Sandy,Daniel Baker</t>
-  </si>
-  <si>
-    <t>John Sandy,David Taylor</t>
-  </si>
-  <si>
-    <t>Daniel Baker,John Sandy</t>
-  </si>
-  <si>
-    <t>John Sandy,Kenneth Neal,John Catchings,Sandra Valdez,Brenda Mcbride,Patrick Hooks</t>
-  </si>
-  <si>
-    <t>Javier Diclaudio,Michael Leatherwood</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn,Kenneth Neal,Susan Tilford,Clarence Wilder</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn,John Sandy,Jeremiah Lopez,Kenneth Neal,Rochelle Braithwaite</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn,Crystal Daniel,John Sandy,John Catchings</t>
-  </si>
-  <si>
-    <t>John Sandy,Daniel Baker,Rochelle Braithwaite,Kenneth Neal</t>
-  </si>
-  <si>
-    <t>John Sandy,Jeremiah Lopez,Joseph Dodd,Mary Javier,Ronald Shaver,Waldo Gray</t>
-  </si>
-  <si>
-    <t>John Sandy,Crystal Daniel,Rochelle Braithwaite,Arthur Stockton,John Catchings,John Yates</t>
-  </si>
-  <si>
-    <t>David Taylor,Kevin VanHorn,Joseph Dodd,Gregory Forbis</t>
-  </si>
-  <si>
-    <t>John Sandy,Rochelle Braithwaite,Harry Villaman,Arthur Stockton,Sandra Valdez,Myra Martinez</t>
-  </si>
-  <si>
-    <t>John Sandy,Judy Salgado,Joseph Dodd,Rochelle Braithwaite,Arthur Stockton,John Catchings</t>
-  </si>
-  <si>
-    <t>Kenneth Neal,Clarence Wilder,Mary Javier,Ronald Shaver,Waldo Gray,David Whapham</t>
+    <t>John Sandy,John Yates,John Catchings,Rochelle Braithwaite,Arthur Stockton,Crystal Daniel</t>
+  </si>
+  <si>
+    <t>Stephanie Sorenson,Sean Richardson</t>
+  </si>
+  <si>
+    <t>John Sandy,Rochelle Braithwaite,Harry Villaman,Arthur Stockton,Myra Martinez,Sandra Valdez</t>
+  </si>
+  <si>
+    <t>John Sandy,Judy Salgado,John Catchings,Gerald Potter,Rochelle Braithwaite,Arthur Stockton</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn,Helen Humphreys,John Sandy,Annemarie Coke,Holly Reed</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn,John Sandy,Susan Tilford,Gregory Forbis,Arthur Stockton</t>
+  </si>
+  <si>
+    <t>Paul Meier,John Sandy</t>
+  </si>
+  <si>
+    <t>Arthur Stockton,Paul Meier</t>
+  </si>
+  <si>
+    <t>Arthur Stockton,John Sandy</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn,John Sandy</t>
+  </si>
+  <si>
+    <t>John Sandy,Brenda Mcbride</t>
+  </si>
+  <si>
+    <t>Rochelle Braithwaite,Mary Javier,Kenneth Neal,John Sandy</t>
+  </si>
+  <si>
+    <t>Rochelle Braithwaite,Mary Javier,Gordon Garcia,Kenneth Neal</t>
+  </si>
+  <si>
+    <t>Waldo Gray,David Whapham,Brenda Mcbride,Ronald Shaver,Jeremiah Lopez,Joseph Dodd</t>
+  </si>
+  <si>
+    <t>Waldo Gray,Clarence Wilder,David Whapham,Ronald Shaver,Arthur Stockton,Mary Javier</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn,David Taylor,Helen Humphreys,Joseph Dodd</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn,Susan Tilford,Helen Humphreys,John Sandy</t>
   </si>
 </sst>
 </file>
@@ -2584,8 +2587,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7981,8 +7984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A021EA-029D-4E52-9D29-4D539B994A79}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8492,10 +8495,10 @@
         <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="D2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8506,7 +8509,7 @@
         <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
       <c r="D3" t="s">
         <v>546</v>
@@ -8520,10 +8523,10 @@
         <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>623</v>
+        <v>612</v>
       </c>
       <c r="D4" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8534,7 +8537,7 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8545,7 +8548,7 @@
         <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -8556,7 +8559,7 @@
         <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8567,7 +8570,7 @@
         <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8578,7 +8581,7 @@
         <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8589,7 +8592,7 @@
         <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8600,7 +8603,7 @@
         <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8611,7 +8614,7 @@
         <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8622,10 +8625,7 @@
         <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>617</v>
-      </c>
-      <c r="D16" t="s">
-        <v>334</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -8636,10 +8636,7 @@
         <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>613</v>
-      </c>
-      <c r="D17" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -8650,7 +8647,7 @@
         <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="D19" t="s">
         <v>163</v>
@@ -8664,10 +8661,10 @@
         <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -8678,7 +8675,7 @@
         <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>536</v>
       </c>
       <c r="D22" t="s">
         <v>427</v>
@@ -8692,7 +8689,7 @@
         <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>536</v>
       </c>
       <c r="D23" t="s">
         <v>156</v>
@@ -8706,10 +8703,10 @@
         <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="D25" t="s">
-        <v>403</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -8720,10 +8717,10 @@
         <v>104</v>
       </c>
       <c r="C26" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D26" t="s">
-        <v>412</v>
+        <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -8734,7 +8731,7 @@
         <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -8745,10 +8742,10 @@
         <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="D29" t="s">
-        <v>609</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -8798,9 +8795,9 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
+  <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01LG763KNURG5YXEOIGVFYKVI5JQCZG47R:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly8zNjV1dHNvdXRod2VzdGVybi1teS5zaGFyZXBvaW50LmNvbS86dTovZy9wZXJzb25hbC9hYmlnYWlsX2xld2lzX3V0c291dGh3ZXN0ZXJuX2VkdS9FYlNKdTR1UnlEVkxoVlVkVEFXVGNfRUJ4RXpaczgyNU5ndEE5M1hkTkRxQlpn"/>
+</scriptIds>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8969,9 +8966,9 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
-  <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01LG763KNURG5YXEOIGVFYKVI5JQCZG47R:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly8zNjV1dHNvdXRod2VzdGVybi1teS5zaGFyZXBvaW50LmNvbS86dTovZy9wZXJzb25hbC9hYmlnYWlsX2xld2lzX3V0c291dGh3ZXN0ZXJuX2VkdS9FYlNKdTR1UnlEVkxoVlVkVEFXVGNfRUJ4RXpaczgyNU5ndEE5M1hkTkRxQlpn"/>
-</scriptIds>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8983,18 +8980,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA16BEB-0523-4F04-9A45-82DF970EB511}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B9B7CB-CCDD-4B54-905C-F8BE57B4D8CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51635bf0-3289-44e9-95c5-5505efa9427e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d0eb518e-69e0-47b9-b413-7592cd52f95f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/extensibility/maker/v1.0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9019,9 +9007,18 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B9B7CB-CCDD-4B54-905C-F8BE57B4D8CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA16BEB-0523-4F04-9A45-82DF970EB511}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/extensibility/maker/v1.0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51635bf0-3289-44e9-95c5-5505efa9427e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d0eb518e-69e0-47b9-b413-7592cd52f95f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[Prototype April Deployment] Added template example.
</commit_message>
<xml_diff>
--- a/Clinic Sign-Up Prototype_2.xlsx
+++ b/Clinic Sign-Up Prototype_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\Desktop\Clinics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F86A42A-1519-44F2-BBAB-F9833821E51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12843735-5276-437E-8C0A-9105F2B1DFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="975" yWindow="-120" windowWidth="27945" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="717">
   <si>
     <t>ID</t>
   </si>
@@ -1938,48 +1938,24 @@
     <t>Stephanie Sorenson, Sean Richardson</t>
   </si>
   <si>
-    <t>John Sandy, Judy Salgado, John Catchings, Gerald Potter, Rochelle Braithwaite, Arthur Stockton</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn, John Sandy, Susan Tilford, Gregory Forbis, Arthur Stockton</t>
-  </si>
-  <si>
-    <t>Paul Meier, John Sandy</t>
-  </si>
-  <si>
-    <t>Arthur Stockton, Paul Meier</t>
-  </si>
-  <si>
-    <t>Arthur Stockton, John Sandy</t>
-  </si>
-  <si>
     <t>Joe Kittelson, Melissa Thompson</t>
   </si>
   <si>
     <t>Michele Slade, Michael Leatherwood</t>
   </si>
   <si>
-    <t>John Sandy, Brenda Mcbride</t>
-  </si>
-  <si>
     <t>Michael Leatherwood, Javier Diclaudio</t>
   </si>
   <si>
     <t>Jim Lewis, Glen Riggs, Michele Slade</t>
   </si>
   <si>
-    <t>Rochelle Braithwaite, Mary Javier, Gordon Garcia, Kenneth Neal</t>
-  </si>
-  <si>
     <t>Glen Riggs, Michele Slade, Lester Mcdonald, Gwendolyn Mcvay, Timothy Calloway</t>
   </si>
   <si>
     <t>Patricia Lee, Percy Bubier, Karen Egnew</t>
   </si>
   <si>
-    <t>Sean Richardson, Patricia Lee, Jim Lewis</t>
-  </si>
-  <si>
     <t>Gwendolyn Mcvay, Patricia Lee, Jim Lewis</t>
   </si>
   <si>
@@ -1998,36 +1974,6 @@
     <t>Details_WaitlistTranslator</t>
   </si>
   <si>
-    <t>Joseph Dodd, Sandra Valdez</t>
-  </si>
-  <si>
-    <t>Sandra Valdez, Jeremiah Lopez, Rochelle Braithwaite, Mary Javier, Kenneth Neal</t>
-  </si>
-  <si>
-    <t>Daniel Baker, Patrick Hooks, Brenda Mcbride, John Yates</t>
-  </si>
-  <si>
-    <t>John Sandy, Patrick Hooks, Brenda Mcbride, David Taylor, John Yates, Susan Tilford</t>
-  </si>
-  <si>
-    <t>John Sandy, Daniel Baker, Mary Javier, Patrick Hooks, David Taylor, Susan Tilford</t>
-  </si>
-  <si>
-    <t>Daniel Baker, Patrick Hooks, Brenda Mcbride</t>
-  </si>
-  <si>
-    <t>Daniel Baker, Patrick Hooks</t>
-  </si>
-  <si>
-    <t>Kenneth Neal, Patrick Hooks, John Catchings, Sandra Valdez</t>
-  </si>
-  <si>
-    <t>Rosa Reyes, John Sandy, Arthur Stockton, Pedro Ware, Daniel Baker, Holly Reed</t>
-  </si>
-  <si>
-    <t>Rochelle Braithwaite, Shelby Boyd, Gordon Garcia, John Sandy, Clarence Wilder, Patrick Hooks</t>
-  </si>
-  <si>
     <t>Rochelle Braithwaite, John Sandy, Patrick Hooks</t>
   </si>
   <si>
@@ -2043,63 +1989,21 @@
     <t>Sean Richardson[6][EL]-MS1</t>
   </si>
   <si>
-    <t>John Sandy[1][EL]-MS4, Judy Salgado[1][EL]-MS4, John Catchings[2][EL]-MS2, Gerald Potter[2]-MS4, Rochelle Braithwaite[3][EL]-MS4, Arthur Stockton[6]-MS2</t>
-  </si>
-  <si>
-    <t>Joseph Dodd[7][EL]-MS1, Sandra Valdez[8]-MS1</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn[1][EL]-MS4, John Sandy[2][EL]-MS4, Susan Tilford[2][EL]-MS1, Gregory Forbis[2]-MS0, Arthur Stockton[3]-MS2</t>
-  </si>
-  <si>
-    <t>Sandra Valdez[4]-MS1, Jeremiah Lopez[5][EL]-MS4, Rochelle Braithwaite[7][EL]-MS4, Mary Javier[7][EL]-MS2, Kenneth Neal[7]-MS0</t>
-  </si>
-  <si>
-    <t>Paul Meier[2][EL]-MS2, John Sandy[3][EL]-MS4</t>
-  </si>
-  <si>
-    <t>Daniel Baker[3][EL]-MS4, Patrick Hooks[3]-MS2, Brenda Mcbride[5]-MS2, John Yates[8]-MS4</t>
-  </si>
-  <si>
-    <t>Arthur Stockton[1]-MS2, Paul Meier[2][EL]-MS2</t>
-  </si>
-  <si>
-    <t>John Sandy[3][EL]-MS4, Patrick Hooks[3]-MS2, Brenda Mcbride[5]-MS2, David Taylor[5][EL]-MS1, John Yates[8]-MS4, Susan Tilford[8][EL]-MS1</t>
-  </si>
-  <si>
     <t>Jim Lewis[7][EL]-MS3</t>
   </si>
   <si>
-    <t>John Sandy[3][EL]-MS4, Daniel Baker[3][EL]-MS4, Mary Javier[3][EL]-MS2, Patrick Hooks[3]-MS2, David Taylor[5][EL]-MS1, Susan Tilford[8][EL]-MS1</t>
-  </si>
-  <si>
     <t>Joe Kittelson[5]-MS4</t>
   </si>
   <si>
-    <t>Arthur Stockton[1]-MS2, John Sandy[3][EL]-MS4</t>
-  </si>
-  <si>
-    <t>Daniel Baker[3][EL]-MS4, Patrick Hooks[3]-MS2, Brenda Mcbride[5]-MS2</t>
-  </si>
-  <si>
     <t>Joe Kittelson[5]-MS4, Melissa Thompson[7][EL]-MS2</t>
   </si>
   <si>
-    <t>Daniel Baker[3][EL]-MS4, Patrick Hooks[3]-MS2</t>
-  </si>
-  <si>
     <t>Michele Slade[5][EL]-MS4, Michael Leatherwood[8][EL]-MS0</t>
   </si>
   <si>
     <t>Leanna Hill[5][EL]-MS0</t>
   </si>
   <si>
-    <t>John Sandy[4][EL]-MS4, Brenda Mcbride[4]-MS2</t>
-  </si>
-  <si>
-    <t>Kenneth Neal[5]-MS0, Patrick Hooks[6]-MS2, John Catchings[7][EL]-MS2, Sandra Valdez[7]-MS1</t>
-  </si>
-  <si>
     <t>Michael Leatherwood[6][EL]-MS0, Javier Diclaudio[7][EL]-MS0</t>
   </si>
   <si>
@@ -2109,15 +2013,9 @@
     <t>Jim Lewis[4][EL]-MS3, Glen Riggs[5]-MS2, Michele Slade[6][EL]-MS4</t>
   </si>
   <si>
-    <t>Rochelle Braithwaite[1][EL]-MS4, Mary Javier[1][EL]-MS2, Gordon Garcia[1]-MS0, Kenneth Neal[3]-MS0</t>
-  </si>
-  <si>
     <t>Robert Riddle[1]-MS1</t>
   </si>
   <si>
-    <t>Rosa Reyes[3]-MS0, John Sandy[5][EL]-MS4, Arthur Stockton[7]-MS2, Pedro Ware[7][EL]-MS4, Daniel Baker[8][EL]-MS4, Holly Reed[8]-MS4</t>
-  </si>
-  <si>
     <t>Glen Riggs[5]-MS2, Michele Slade[6][EL]-MS4, Lester Mcdonald[6]-MS3, Gwendolyn Mcvay[6]-MS0, Timothy Calloway[8][EL]-MS3</t>
   </si>
   <si>
@@ -2127,9 +2025,6 @@
     <t>Karen Egnew[7][EL]-MS4</t>
   </si>
   <si>
-    <t>Rochelle Braithwaite[4][EL]-MS4, Shelby Boyd[4][EL]-MS2, Gordon Garcia[5]-MS0, John Sandy[6][EL]-MS4, Clarence Wilder[7]-MS2, Patrick Hooks[7]-MS2</t>
-  </si>
-  <si>
     <t>William Cauley[4][EL]-MS0</t>
   </si>
   <si>
@@ -2142,9 +2037,6 @@
     <t>Heather Favorite[4]-MS0</t>
   </si>
   <si>
-    <t>Sean Richardson[7][EL]-MS1, Patricia Lee[8]-MS1, Jim Lewis[8][EL]-MS3</t>
-  </si>
-  <si>
     <t>Gordon Garcia[8]-MS0</t>
   </si>
   <si>
@@ -2169,51 +2061,15 @@
     <t>Harry Villaman[6]-MS0, John Sandy[1][EL]-MS4, Rochelle Braithwaite[3][EL]-MS4, Arthur Stockton[6]-MS2, Myra Martinez[8][EL]-MS0, Sandra Valdez[8]-MS1</t>
   </si>
   <si>
-    <t>Kevin VanHorn, Helen Humphreys, John Sandy, John Catchings, Sandra Valdez</t>
-  </si>
-  <si>
-    <t>Annemarie Coke, Holly Reed, Jeremiah Lopez, Rochelle Braithwaite, Mary Javier, Kenneth Neal</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn[1][EL]-MS4, Helen Humphreys[1][EL]-MS4, John Sandy[2][EL]-MS4, John Catchings[4][EL]-MS2, Sandra Valdez[4]-MS1</t>
-  </si>
-  <si>
-    <t>Annemarie Coke[3][EL]-MS3, Holly Reed[3]-MS4, Jeremiah Lopez[5][EL]-MS4, Rochelle Braithwaite[7][EL]-MS4, Mary Javier[7][EL]-MS2, Kenneth Neal[7]-MS0</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn, Crystal Daniel</t>
-  </si>
-  <si>
     <t>John Sandy, John Catchings</t>
   </si>
   <si>
-    <t>Kevin VanHorn[2][EL]-MS4, Crystal Daniel[4][EL]-MS2</t>
-  </si>
-  <si>
     <t>John Sandy[4][EL]-MS4, John Catchings[7][EL]-MS2</t>
   </si>
   <si>
-    <t>Rochelle Braithwaite, Mary Javier, John Sandy, John Catchings</t>
-  </si>
-  <si>
-    <t>Kenneth Neal, Arthur Stockton, Pedro Ware, Daniel Baker, Holly Reed</t>
-  </si>
-  <si>
-    <t>Rochelle Braithwaite[1][EL]-MS4, Mary Javier[1][EL]-MS2, John Sandy[5][EL]-MS4, John Catchings[5][EL]-MS2</t>
-  </si>
-  <si>
-    <t>Kenneth Neal[3]-MS0, Arthur Stockton[7]-MS2, Pedro Ware[7][EL]-MS4, Daniel Baker[8][EL]-MS4, Holly Reed[8]-MS4</t>
-  </si>
-  <si>
-    <t>Jeremiah Lopez, Helen Humphreys, Waldo Gray, David Whapham, Brenda Mcbride, Ronald Shaver</t>
-  </si>
-  <si>
     <t>Joseph Dodd, Mary Javier, Kenneth Neal</t>
   </si>
   <si>
-    <t>Jeremiah Lopez[3][EL]-MS4, Helen Humphreys[7][EL]-MS4, Waldo Gray[2]-MS1, David Whapham[2]-MS2, Brenda Mcbride[2]-MS2, Ronald Shaver[3]-MS3</t>
-  </si>
-  <si>
     <t>Joseph Dodd[5][EL]-MS1, Mary Javier[5][EL]-MS2, Kenneth Neal[8]-MS0</t>
   </si>
   <si>
@@ -2223,10 +2079,178 @@
     <t>Waldo Gray[2]-MS1, Clarence Wilder[2]-MS2, Ronald Shaver[3]-MS3, Kenneth Neal[8]-MS0, David Whapham[2]-MS2, Mary Javier[5][EL]-MS2</t>
   </si>
   <si>
-    <t>Kevin VanHorn, Susan Tilford, John Sandy</t>
-  </si>
-  <si>
-    <t>Kevin VanHorn[3][EL]-MS4, Susan Tilford[4][EL]-MS1, John Sandy[7][EL]-MS4</t>
+    <t>Stephanie Sorenson, Phyllis Davis</t>
+  </si>
+  <si>
+    <t>Arthur Stockton, Sandra Valdez</t>
+  </si>
+  <si>
+    <t>Stephanie Sorenson[5]-MS3, Phyllis Davis[7][EL]-MS2</t>
+  </si>
+  <si>
+    <t>Arthur Stockton[6]-MS2, Sandra Valdez[8]-MS1</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn, Helen Humphreys, Annemarie Coke, Sandra Valdez, John Catchings</t>
+  </si>
+  <si>
+    <t>Kevin VanHorn[1][EL]-MS4, Helen Humphreys[1][EL]-MS4, Annemarie Coke[3][EL]-MS3, Sandra Valdez[4]-MS1, John Catchings[4][EL]-MS2</t>
+  </si>
+  <si>
+    <t>Paul Meier, Daniel Baker</t>
+  </si>
+  <si>
+    <t>Patrick Hooks, Brenda Mcbride, John Sandy, John Yates</t>
+  </si>
+  <si>
+    <t>Paul Meier[2][EL]-MS2, Daniel Baker[3][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Patrick Hooks[3]-MS2, Brenda Mcbride[5]-MS2, John Sandy[3][EL]-MS4, John Yates[8]-MS4</t>
+  </si>
+  <si>
+    <t>Arthur Stockton, Patrick Hooks</t>
+  </si>
+  <si>
+    <t>Arthur Stockton[1]-MS2, Patrick Hooks[3]-MS2</t>
+  </si>
+  <si>
+    <t>Patrick Hooks, John Sandy</t>
+  </si>
+  <si>
+    <t>Patrick Hooks[3]-MS2, John Sandy[3][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Brenda Mcbride, Kenneth Neal</t>
+  </si>
+  <si>
+    <t>John Sandy, Sandra Valdez, Patrick Hooks, John Catchings</t>
+  </si>
+  <si>
+    <t>Brenda Mcbride[4]-MS2, Kenneth Neal[5]-MS0</t>
+  </si>
+  <si>
+    <t>John Sandy[4][EL]-MS4, Sandra Valdez[7]-MS1, Patrick Hooks[6]-MS2, John Catchings[7][EL]-MS2</t>
+  </si>
+  <si>
+    <t>Mary Javier, Rochelle Braithwaite, Pedro Ware, John Catchings</t>
+  </si>
+  <si>
+    <t>Kenneth Neal, Holly Reed, John Sandy, Daniel Baker, Arthur Stockton</t>
+  </si>
+  <si>
+    <t>Mary Javier[1][EL]-MS2, Rochelle Braithwaite[1][EL]-MS4, Pedro Ware[7][EL]-MS4, John Catchings[5][EL]-MS2</t>
+  </si>
+  <si>
+    <t>Kenneth Neal[3]-MS0, Holly Reed[8]-MS4, John Sandy[5][EL]-MS4, Daniel Baker[8][EL]-MS4, Arthur Stockton[7]-MS2</t>
+  </si>
+  <si>
+    <t>Shelby Boyd, Gordon Garcia, Clarence Wilder, Rochelle Braithwaite, John Sandy, Patrick Hooks</t>
+  </si>
+  <si>
+    <t>Shelby Boyd[4][EL]-MS2, Gordon Garcia[5]-MS0, Clarence Wilder[7]-MS2, Rochelle Braithwaite[4][EL]-MS4, John Sandy[6][EL]-MS4, Patrick Hooks[7]-MS2</t>
+  </si>
+  <si>
+    <t>Patricia Lee, Jim Lewis, Sean Richardson</t>
+  </si>
+  <si>
+    <t>Patricia Lee[8]-MS1, Jim Lewis[8][EL]-MS3, Sean Richardson[7][EL]-MS1</t>
+  </si>
+  <si>
+    <t>Susan Tilford, Kevin VanHorn, John Sandy</t>
+  </si>
+  <si>
+    <t>Susan Tilford[4][EL]-MS1, Kevin VanHorn[3][EL]-MS4, John Sandy[7][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Judy Salgado, Gerald Potter, John Catchings, John Sandy, Rochelle Braithwaite, Joseph Dodd</t>
+  </si>
+  <si>
+    <t>Judy Salgado[1][EL]-MS4, Gerald Potter[2]-MS4, John Catchings[2][EL]-MS2, John Sandy[1][EL]-MS4, Rochelle Braithwaite[3][EL]-MS4, Joseph Dodd[7][EL]-MS1</t>
+  </si>
+  <si>
+    <t>Holly Reed, Jeremiah Lopez, John Sandy, Mary Javier, Kenneth Neal, Rochelle Braithwaite</t>
+  </si>
+  <si>
+    <t>Holly Reed[3]-MS4, Jeremiah Lopez[5][EL]-MS4, John Sandy[2][EL]-MS4, Mary Javier[7][EL]-MS2, Kenneth Neal[7]-MS0, Rochelle Braithwaite[7][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Susan Tilford, Gregory Forbis, Kevin VanHorn, Jeremiah Lopez, Arthur Stockton</t>
+  </si>
+  <si>
+    <t>John Sandy, Sandra Valdez, Mary Javier, Kenneth Neal, Rochelle Braithwaite</t>
+  </si>
+  <si>
+    <t>Susan Tilford[2][EL]-MS1, Gregory Forbis[2]-MS0, Kevin VanHorn[1][EL]-MS4, Jeremiah Lopez[5][EL]-MS4, Arthur Stockton[3]-MS2</t>
+  </si>
+  <si>
+    <t>John Sandy[2][EL]-MS4, Sandra Valdez[4]-MS1, Mary Javier[7][EL]-MS2, Kenneth Neal[7]-MS0, Rochelle Braithwaite[7][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Patrick Hooks, Paul Meier</t>
+  </si>
+  <si>
+    <t>Brenda Mcbride, Arthur Stockton, David Taylor, John Sandy, John Yates, Susan Tilford</t>
+  </si>
+  <si>
+    <t>Patrick Hooks[3]-MS2, Paul Meier[2][EL]-MS2</t>
+  </si>
+  <si>
+    <t>Brenda Mcbride[5]-MS2, Arthur Stockton[1]-MS2, David Taylor[5][EL]-MS1, John Sandy[3][EL]-MS4, John Yates[8]-MS4, Susan Tilford[8][EL]-MS1</t>
+  </si>
+  <si>
+    <t>Daniel Baker, Mary Javier</t>
+  </si>
+  <si>
+    <t>Patrick Hooks, Paul Meier, Arthur Stockton, David Taylor, John Sandy, Susan Tilford</t>
+  </si>
+  <si>
+    <t>Daniel Baker[3][EL]-MS4, Mary Javier[3][EL]-MS2</t>
+  </si>
+  <si>
+    <t>Patrick Hooks[3]-MS2, Paul Meier[2][EL]-MS2, Arthur Stockton[1]-MS2, David Taylor[5][EL]-MS1, John Sandy[3][EL]-MS4, Susan Tilford[8][EL]-MS1</t>
+  </si>
+  <si>
+    <t>John Sandy, Daniel Baker</t>
+  </si>
+  <si>
+    <t>John Sandy[3][EL]-MS4, Daniel Baker[3][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Crystal Daniel, Kevin VanHorn</t>
+  </si>
+  <si>
+    <t>Crystal Daniel[4][EL]-MS2, Kevin VanHorn[2][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Jeremiah Lopez, Helen Humphreys, Waldo Gray, David Whapham, Ronald Shaver, Brenda Mcbride</t>
+  </si>
+  <si>
+    <t>Jeremiah Lopez[3][EL]-MS4, Helen Humphreys[7][EL]-MS4, Waldo Gray[2]-MS1, David Whapham[2]-MS2, Ronald Shaver[3]-MS3, Brenda Mcbride[2]-MS2</t>
+  </si>
+  <si>
+    <t>Patrick Hooks, Brenda Mcbride</t>
+  </si>
+  <si>
+    <t>Arthur Stockton, Daniel Baker, John Sandy</t>
+  </si>
+  <si>
+    <t>Patrick Hooks[3]-MS2, Brenda Mcbride[5]-MS2</t>
+  </si>
+  <si>
+    <t>Arthur Stockton[1]-MS2, Daniel Baker[3][EL]-MS4, John Sandy[3][EL]-MS4</t>
+  </si>
+  <si>
+    <t>Gordon Garcia, Rosa Reyes, Mary Javier, Kenneth Neal</t>
+  </si>
+  <si>
+    <t>Rochelle Braithwaite, Holly Reed, Pedro Ware, John Sandy, Daniel Baker, Arthur Stockton</t>
+  </si>
+  <si>
+    <t>Gordon Garcia[1]-MS0, Rosa Reyes[3]-MS0, Mary Javier[1][EL]-MS2, Kenneth Neal[3]-MS0</t>
+  </si>
+  <si>
+    <t>Rochelle Braithwaite[1][EL]-MS4, Holly Reed[8]-MS4, Pedro Ware[7][EL]-MS4, John Sandy[5][EL]-MS4, Daniel Baker[8][EL]-MS4, Arthur Stockton[7]-MS2</t>
   </si>
 </sst>
 </file>
@@ -2430,7 +2454,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2491,51 +2515,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2555,19 +2541,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{129FA3A9-BD6A-43A7-967D-34493BA52639}" name="Table3" displayName="Table3" ref="A1:J30" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:J30" xr:uid="{129FA3A9-BD6A-43A7-967D-34493BA52639}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F0A78D4A-361F-491E-9D59-CEBC77C07E55}" name="Table2" displayName="Table2" ref="A1:J29" totalsRowShown="0">
+  <autoFilter ref="A1:J29" xr:uid="{F0A78D4A-361F-491E-9D59-CEBC77C07E55}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{495AAC11-C051-4ACC-80A7-911071B7FCA9}" name="Clinic" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{378AC0EF-94FB-46CD-8E75-874B87A75966}" name="Date" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{CF921308-3943-4EAD-A42C-AC7739C411C3}" name="Volunteers" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{964DF9F4-49A2-40D7-B6C9-ADFF5BFE19DC}" name="Translators" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{4DE0C122-11BD-436E-9472-D3E902603D6E}" name="Waitlist-General" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{3562717B-3712-445C-93A3-B86ACAF2DE2F}" name="Waitlist-Translator" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{289DA763-B416-4F7E-B71D-CBA18E38D2A0}" name="Details_Volunteer" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{821FAFF1-1816-438F-9444-2423D26E38B1}" name="Details_Translators" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{3CBA062C-5253-48CD-8DD5-205FF2FBB10A}" name="Details_WaitlistGeneral" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{8B0781DE-2DBC-470C-8837-A642E83797A5}" name="Details_WaitlistTranslator" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{BEE767F8-E7A8-4383-ADC7-9267EAFC90F7}" name="Clinic"/>
+    <tableColumn id="2" xr3:uid="{45B472A3-5EF3-4D40-A6FA-7D2C9859BFB3}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{6735A3B5-8F28-436D-AB58-2FD07759D40F}" name="Volunteers"/>
+    <tableColumn id="4" xr3:uid="{541ED32C-869E-4560-9A6E-7CE5FF69A0E0}" name="Translators"/>
+    <tableColumn id="5" xr3:uid="{79F1DD0A-D2B9-41CC-B7E2-8E9D2052A26C}" name="Waitlist-General"/>
+    <tableColumn id="6" xr3:uid="{FE0307B3-8FB2-4E43-90F5-E4E0EF27AF32}" name="Waitlist-Translator"/>
+    <tableColumn id="7" xr3:uid="{8F07810F-0292-445C-A35F-296BE650DC8A}" name="Details_Volunteer"/>
+    <tableColumn id="8" xr3:uid="{436F301E-31C0-4223-95B1-460DA17C9020}" name="Details_Translators"/>
+    <tableColumn id="9" xr3:uid="{FF2D2432-E57D-44F1-91E9-389526CB8425}" name="Details_WaitlistGeneral"/>
+    <tableColumn id="10" xr3:uid="{5F67CB44-7A09-42EC-9BC9-02DC8837A807}" name="Details_WaitlistTranslator"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2897,7 +2883,7 @@
   <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8293,8 +8279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A021EA-029D-4E52-9D29-4D539B994A79}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8798,11 +8784,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C53F42-3A8C-4FFB-9E26-236D3EB50430}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8814,7 +8800,7 @@
     <col min="5" max="5" width="88.85546875" style="23" customWidth="1"/>
     <col min="6" max="6" width="41.5703125" style="23" customWidth="1"/>
     <col min="7" max="7" width="98.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" style="23" customWidth="1"/>
+    <col min="8" max="8" width="47" style="23" customWidth="1"/>
     <col min="9" max="9" width="97.140625" style="23" customWidth="1"/>
     <col min="10" max="10" width="106.85546875" style="23" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="23"/>
@@ -8834,10 +8820,10 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="F1" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="G1" t="s">
         <v>609</v>
@@ -8846,10 +8832,10 @@
         <v>610</v>
       </c>
       <c r="I1" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="J1" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -8860,7 +8846,7 @@
         <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>685</v>
+        <v>649</v>
       </c>
       <c r="D2" t="s">
         <v>611</v>
@@ -8872,16 +8858,16 @@
         <v>503</v>
       </c>
       <c r="G2" t="s">
-        <v>686</v>
+        <v>650</v>
       </c>
       <c r="H2" t="s">
-        <v>643</v>
+        <v>625</v>
       </c>
       <c r="I2" t="s">
-        <v>644</v>
+        <v>626</v>
       </c>
       <c r="J2" t="s">
-        <v>645</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8892,7 +8878,7 @@
         <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>687</v>
+        <v>651</v>
       </c>
       <c r="D3" t="s">
         <v>546</v>
@@ -8900,10 +8886,10 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="s">
-        <v>688</v>
+        <v>652</v>
       </c>
       <c r="H3" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -8916,28 +8902,28 @@
         <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>612</v>
+        <v>687</v>
       </c>
       <c r="D4" t="s">
-        <v>611</v>
+        <v>659</v>
       </c>
       <c r="E4" t="s">
-        <v>632</v>
+        <v>660</v>
       </c>
       <c r="F4" t="s">
-        <v>503</v>
+        <v>546</v>
       </c>
       <c r="G4" t="s">
-        <v>647</v>
+        <v>688</v>
       </c>
       <c r="H4" t="s">
-        <v>643</v>
+        <v>661</v>
       </c>
       <c r="I4" t="s">
-        <v>648</v>
+        <v>662</v>
       </c>
       <c r="J4" t="s">
-        <v>645</v>
+        <v>628</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -8960,19 +8946,19 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>689</v>
+        <v>663</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>691</v>
+        <v>664</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="J6"/>
     </row>
@@ -8984,19 +8970,19 @@
         <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>613</v>
+        <v>691</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>633</v>
+        <v>692</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
-        <v>649</v>
+        <v>693</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>650</v>
+        <v>694</v>
       </c>
       <c r="J7"/>
     </row>
@@ -9020,19 +9006,19 @@
         <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>614</v>
+        <v>665</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>634</v>
+        <v>666</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>651</v>
+        <v>667</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>652</v>
+        <v>668</v>
       </c>
       <c r="J9"/>
     </row>
@@ -9044,24 +9030,24 @@
         <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>615</v>
+        <v>695</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>635</v>
+        <v>696</v>
       </c>
       <c r="F10" t="s">
         <v>403</v>
       </c>
       <c r="G10" t="s">
-        <v>653</v>
+        <v>697</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="s">
-        <v>654</v>
+        <v>698</v>
       </c>
       <c r="J10" t="s">
-        <v>655</v>
+        <v>629</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -9072,24 +9058,24 @@
         <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>615</v>
+        <v>699</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>636</v>
+        <v>700</v>
       </c>
       <c r="F11" t="s">
         <v>289</v>
       </c>
       <c r="G11" t="s">
-        <v>653</v>
+        <v>701</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="s">
-        <v>656</v>
+        <v>702</v>
       </c>
       <c r="J11" t="s">
-        <v>657</v>
+        <v>630</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -9100,24 +9086,24 @@
         <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>616</v>
+        <v>709</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>637</v>
+        <v>710</v>
       </c>
       <c r="F12" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="G12" t="s">
-        <v>658</v>
+        <v>711</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="s">
-        <v>659</v>
+        <v>712</v>
       </c>
       <c r="J12" t="s">
-        <v>660</v>
+        <v>631</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -9128,24 +9114,24 @@
         <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>614</v>
+        <v>665</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>638</v>
+        <v>671</v>
       </c>
       <c r="F13" t="s">
         <v>289</v>
       </c>
       <c r="G13" t="s">
-        <v>651</v>
+        <v>667</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>661</v>
+        <v>672</v>
       </c>
       <c r="J13" t="s">
-        <v>657</v>
+        <v>630</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -9156,24 +9142,24 @@
         <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>616</v>
+        <v>669</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>638</v>
+        <v>703</v>
       </c>
       <c r="F14" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="G14" t="s">
-        <v>658</v>
+        <v>670</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>661</v>
+        <v>704</v>
       </c>
       <c r="J14" t="s">
-        <v>662</v>
+        <v>632</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -9196,24 +9182,24 @@
         <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>693</v>
+        <v>705</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>694</v>
+        <v>653</v>
       </c>
       <c r="F16" t="s">
         <v>334</v>
       </c>
       <c r="G16" t="s">
-        <v>695</v>
+        <v>706</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>696</v>
+        <v>654</v>
       </c>
       <c r="J16" t="s">
-        <v>663</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -9224,24 +9210,24 @@
         <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>619</v>
+        <v>673</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>639</v>
+        <v>674</v>
       </c>
       <c r="F17" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="G17" t="s">
-        <v>664</v>
+        <v>675</v>
       </c>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="J17" t="s">
-        <v>666</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -9264,28 +9250,28 @@
         <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>697</v>
+        <v>677</v>
       </c>
       <c r="D19" t="s">
         <v>163</v>
       </c>
       <c r="E19" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
       <c r="F19" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G19" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="H19" t="s">
-        <v>667</v>
+        <v>635</v>
       </c>
       <c r="I19" t="s">
-        <v>700</v>
+        <v>680</v>
       </c>
       <c r="J19" t="s">
-        <v>668</v>
+        <v>636</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -9296,28 +9282,28 @@
         <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>622</v>
+        <v>713</v>
       </c>
       <c r="D20" t="s">
         <v>352</v>
       </c>
       <c r="E20" t="s">
-        <v>640</v>
+        <v>714</v>
       </c>
       <c r="F20" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="G20" t="s">
-        <v>669</v>
+        <v>715</v>
       </c>
       <c r="H20" t="s">
-        <v>670</v>
+        <v>637</v>
       </c>
       <c r="I20" t="s">
-        <v>671</v>
+        <v>716</v>
       </c>
       <c r="J20" t="s">
-        <v>672</v>
+        <v>638</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -9346,17 +9332,17 @@
         <v>427</v>
       </c>
       <c r="E22" t="s">
-        <v>641</v>
+        <v>681</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="s">
-        <v>673</v>
+        <v>639</v>
       </c>
       <c r="H22" t="s">
-        <v>674</v>
+        <v>640</v>
       </c>
       <c r="I22" t="s">
-        <v>675</v>
+        <v>682</v>
       </c>
       <c r="J22"/>
     </row>
@@ -9374,22 +9360,22 @@
         <v>156</v>
       </c>
       <c r="E23" t="s">
+        <v>624</v>
+      </c>
+      <c r="F23" t="s">
+        <v>617</v>
+      </c>
+      <c r="G23" t="s">
+        <v>639</v>
+      </c>
+      <c r="H23" t="s">
+        <v>641</v>
+      </c>
+      <c r="I23" t="s">
         <v>642</v>
       </c>
-      <c r="F23" t="s">
-        <v>624</v>
-      </c>
-      <c r="G23" t="s">
-        <v>673</v>
-      </c>
-      <c r="H23" t="s">
-        <v>676</v>
-      </c>
-      <c r="I23" t="s">
-        <v>677</v>
-      </c>
       <c r="J23" t="s">
-        <v>678</v>
+        <v>643</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -9412,28 +9398,28 @@
         <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="D25" t="s">
         <v>440</v>
       </c>
       <c r="E25" t="s">
-        <v>702</v>
+        <v>655</v>
       </c>
       <c r="F25" t="s">
-        <v>625</v>
+        <v>683</v>
       </c>
       <c r="G25" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="H25" t="s">
-        <v>679</v>
+        <v>644</v>
       </c>
       <c r="I25" t="s">
-        <v>704</v>
+        <v>656</v>
       </c>
       <c r="J25" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -9444,7 +9430,7 @@
         <v>104</v>
       </c>
       <c r="C26" t="s">
-        <v>705</v>
+        <v>657</v>
       </c>
       <c r="D26" t="s">
         <v>440</v>
@@ -9453,19 +9439,19 @@
         <v>560</v>
       </c>
       <c r="F26" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="G26" t="s">
-        <v>706</v>
+        <v>658</v>
       </c>
       <c r="H26" t="s">
-        <v>679</v>
+        <v>644</v>
       </c>
       <c r="I26" t="s">
-        <v>681</v>
+        <v>645</v>
       </c>
       <c r="J26" t="s">
-        <v>682</v>
+        <v>646</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -9488,13 +9474,13 @@
         <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="s">
-        <v>683</v>
+        <v>647</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
@@ -9508,7 +9494,7 @@
         <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>707</v>
+        <v>685</v>
       </c>
       <c r="D29" t="s">
         <v>503</v>
@@ -9516,50 +9502,132 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="s">
-        <v>708</v>
+        <v>686</v>
       </c>
       <c r="H29" t="s">
-        <v>684</v>
+        <v>648</v>
       </c>
       <c r="I29"/>
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100037D8141F98A5E4B81E16549BD24B904" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff3f115fe85014f51f3f545a574f572d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="51635bf0-3289-44e9-95c5-5505efa9427e" xmlns:ns3="d0eb518e-69e0-47b9-b413-7592cd52f95f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9da3ea708f3e05eff99224ea1dd1a8e2" ns2:_="" ns3:_="">
     <xsd:import namespace="51635bf0-3289-44e9-95c5-5505efa9427e"/>
@@ -9724,6 +9792,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
   <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01LG763KNURG5YXEOIGVFYKVI5JQCZG47R:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly8zNjV1dHNvdXRod2VzdGVybi1teS5zaGFyZXBvaW50LmNvbS86dTovZy9wZXJzb25hbC9hYmlnYWlsX2xld2lzX3V0c291dGh3ZXN0ZXJuX2VkdS9FYlNKdTR1UnlEVkxoVlVkVEFXVGNfRUJ4RXpaczgyNU5ndEE5M1hkTkRxQlpn"/>
@@ -9731,9 +9814,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63981BB9-060E-4857-8C4B-83421E3C53E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2572CB0B-2263-4ABB-8F71-C2290B63E0E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="51635bf0-3289-44e9-95c5-5505efa9427e"/>
+    <ds:schemaRef ds:uri="d0eb518e-69e0-47b9-b413-7592cd52f95f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9756,20 +9850,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2572CB0B-2263-4ABB-8F71-C2290B63E0E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63981BB9-060E-4857-8C4B-83421E3C53E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="51635bf0-3289-44e9-95c5-5505efa9427e"/>
-    <ds:schemaRef ds:uri="d0eb518e-69e0-47b9-b413-7592cd52f95f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>